<commit_message>
Add: quests and journal entries
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E1C821-4266-485D-8754-599799D81EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458CA9C5-63E8-4F8F-B150-429D5B9345CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="6" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Greeting 5</t>
   </si>
   <si>
-    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say Aeliana is currently out. Wait, are you heading out into the wilderness? If you are could you please let my foolish wife know that her wife is worried.</t>
-  </si>
-  <si>
     <t>Journal "tlvoea_Errant_Wife", 11</t>
   </si>
   <si>
@@ -419,6 +416,15 @@
   </si>
   <si>
     <t>Urtiso's House Key</t>
+  </si>
+  <si>
+    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are could you please let my foolish wife know that her wife is worried.</t>
+  </si>
+  <si>
+    <t>Service Refusal</t>
+  </si>
+  <si>
+    <t>I'd be happy to do business with you %PCName, but I need to be back home where my gold and goods are before we can trade.</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1403,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1582,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
@@ -1591,7 +1597,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1599,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1608,7 +1614,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1616,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1630,13 +1636,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1644,13 +1650,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1922,15 +1928,15 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1938,10 +1944,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1949,10 +1955,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2015,7 +2021,7 @@
   <dimension ref="A2:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2040,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -2045,13 +2051,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2212,7 +2218,7 @@
   <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2241,7 +2247,7 @@
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -2261,7 +2267,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -2281,7 +2287,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -2298,7 +2304,7 @@
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -2318,7 +2324,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -2338,13 +2344,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>300</v>
@@ -2358,19 +2364,19 @@
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -2539,10 +2545,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F104"/>
+  <dimension ref="A2:F105"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2581,10 +2587,10 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2598,10 +2604,10 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2615,10 +2621,10 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2632,10 +2638,10 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2649,13 +2655,13 @@
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2669,36 +2675,33 @@
         <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
         <v>0</v>
       </c>
@@ -2706,16 +2709,19 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>78</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
         <v>0</v>
       </c>
@@ -2723,19 +2729,16 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
         <v>0</v>
       </c>
@@ -2743,36 +2746,36 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
         <v>0</v>
       </c>
@@ -2780,16 +2783,19 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="b">
         <v>0</v>
       </c>
@@ -2797,19 +2803,16 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="b">
         <v>0</v>
       </c>
@@ -2817,16 +2820,16 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2834,38 +2837,53 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="2" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -3293,8 +3311,13 @@
         <v>0</v>
       </c>
     </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F104">
+  <conditionalFormatting sqref="B3:F105">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -3727,7 +3750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65134921-D347-4BBE-A2AC-6E1606FA8DED}">
   <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -3767,13 +3790,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3781,13 +3804,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" t="s">
         <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3795,13 +3818,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
         <v>85</v>
       </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3982,10 +4005,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
         <v>118</v>
-      </c>
-      <c r="C3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4179,10 +4202,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
         <v>120</v>
-      </c>
-      <c r="C3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add: most quest dialogue
Add: rent tracking global script
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25054E7B-364B-4F6C-8A72-C62C7FD8A525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B79272-7699-4654-8539-F23481DB58E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="156">
   <si>
     <t>Name</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Wonderful! My house is just outside Old Ebonheart. You can't miss it as it's just a little ways down the road from the gate. I don't know which way that is. I normally just stand on a tall hill to spot the walls.</t>
   </si>
   <si>
-    <t>8, -21</t>
-  </si>
-  <si>
     <t>Oh ok. Maybe I'll be able to make my way back.</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>Faustus' Spare Room Key</t>
   </si>
   <si>
-    <t>Have you found my wife?</t>
-  </si>
-  <si>
     <t>Journal "tlvoea_Errant_Wife", 20; Goodbye</t>
   </si>
   <si>
@@ -376,15 +370,6 @@
     <t>short</t>
   </si>
   <si>
-    <t>tlvoea_Rent_Total</t>
-  </si>
-  <si>
-    <t>tlvoea_Rent_Amount</t>
-  </si>
-  <si>
-    <t>tlvoea_Rent_Period</t>
-  </si>
-  <si>
     <t>Every Rent_Period add Rent_Amount to Rent_Total</t>
   </si>
   <si>
@@ -425,6 +410,111 @@
   </si>
   <si>
     <t>Aeliana? Oh Urtiso's wife. I last saw her somewhere around Haliwaran. Just head a little east down this ridge and it will be in front of you.</t>
+  </si>
+  <si>
+    <t>9, -21</t>
+  </si>
+  <si>
+    <t>*Squeek*</t>
+  </si>
+  <si>
+    <t>*Squeek* *Squeek*</t>
+  </si>
+  <si>
+    <t>[She sniffs the air.]</t>
+  </si>
+  <si>
+    <t>[She sniffs your hand.]</t>
+  </si>
+  <si>
+    <t>Random100 &lt; 75</t>
+  </si>
+  <si>
+    <t>Random100 &lt; 10</t>
+  </si>
+  <si>
+    <t>Random100 &lt; 15</t>
+  </si>
+  <si>
+    <t>Talked to PC == 0, tlvoea_Errant_Wife.Journal &lt; 10</t>
+  </si>
+  <si>
+    <t>My wife is still out, and so the shop remains closed.</t>
+  </si>
+  <si>
+    <t>Have you found Aeliana?</t>
+  </si>
+  <si>
+    <t>AddTopic "spare room"; Journal "tlvoea_Errant_Wife", 100</t>
+  </si>
+  <si>
+    <t>I hope you're better with finding your way round than I am.</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &lt; 20, tlvoea_isAelianaHome == 0</t>
+  </si>
+  <si>
+    <t>spare room</t>
+  </si>
+  <si>
+    <t>Choice "I'll take it.", 1, "No thank you.", 2</t>
+  </si>
+  <si>
+    <t>tlvoea_Spare_Room.Journal &lt; 10</t>
+  </si>
+  <si>
+    <t>I think having you stay with us would be wonderful!</t>
+  </si>
+  <si>
+    <t>Good, here's your key. It's upstairs and at the end of the landing. As for your rent please come to me to pay it, but don't worry about needing to do so everyday. I understand that you're a busy %PCClass, so I'll keep track of what you owe between visits.</t>
+  </si>
+  <si>
+    <t>Not a problem. If you change your mind do speak to me again.</t>
+  </si>
+  <si>
+    <t>I hope it's to your liking.</t>
+  </si>
+  <si>
+    <t>tlvoea_Spare_Room.Journal &gt;= 10</t>
+  </si>
+  <si>
+    <t>AddTopic "room rent"; RemoveItem "tlvoea_faustus_spare_room_key", 1; Player-&gt;AddItem "tlvoea_faustus_spare_room_key", 1; Journal "tlvoea_Spare_Room", 10; StartScript "tlvoea_renting_glb_script"</t>
+  </si>
+  <si>
+    <t>I'm very happy that you've decided to stay with us.</t>
+  </si>
+  <si>
+    <t>I hope hope it suits you.</t>
+  </si>
+  <si>
+    <t>tlvoea_Spare_Room.Journal &gt;= 10; Random100 &lt; 55</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &gt; 11, tlvoea_Errant_Wife.Journal &lt; 20, Random100 &lt; 45</t>
+  </si>
+  <si>
+    <t>I hope she's alright.</t>
+  </si>
+  <si>
+    <t>tlvoea_Glob_Rent_Period</t>
+  </si>
+  <si>
+    <t>tlvoea_Glob_Rent_Price</t>
+  </si>
+  <si>
+    <t>tlvoea_Glob_Rent_Counter</t>
+  </si>
+  <si>
+    <t>It's not much, but it's yours for 15 gold every 2 days. It has a bed, side table, chest and candle.</t>
+  </si>
+  <si>
+    <t>room rent</t>
+  </si>
+  <si>
+    <t>This is what you owe.</t>
+  </si>
+  <si>
+    <t>MessageBox "You owe %G gold.", tlvoea_Glob_Rent_Counter</t>
   </si>
 </sst>
 </file>
@@ -1340,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B451BEBD-3E4F-477C-8824-662D4D8A357C}">
   <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,7 +1484,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1403,7 +1493,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1559,7 +1649,7 @@
   <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
@@ -1597,7 +1687,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1605,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1614,7 +1704,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1622,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1636,27 +1726,27 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1911,12 +2001,12 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1928,15 +2018,15 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1944,24 +2034,24 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2054,10 +2144,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2350,7 +2440,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D8">
         <v>300</v>
@@ -2367,16 +2457,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -2545,10 +2635,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F105"/>
+  <dimension ref="A2:F116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2587,13 +2677,13 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
         <v>1</v>
       </c>
@@ -2604,10 +2694,10 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2621,50 +2711,50 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
         <v>1</v>
       </c>
@@ -2675,13 +2765,10 @@
         <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2692,33 +2779,33 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2726,73 +2813,70 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>64</v>
+        <v>88</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2800,19 +2884,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="b">
         <v>1</v>
       </c>
@@ -2820,213 +2901,408 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
         <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>101</v>
+        <v>59</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="b">
         <v>0</v>
       </c>
@@ -3316,8 +3592,63 @@
         <v>0</v>
       </c>
     </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F105">
+  <conditionalFormatting sqref="B3:F116">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -3751,7 +4082,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3790,13 +4121,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3804,13 +4135,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3818,13 +4149,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -4005,10 +4336,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4202,10 +4533,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix: dialogue greetin not triggering when escorting Aeliana
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B79272-7699-4654-8539-F23481DB58E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0494618-3877-4A30-B1D3-2A29D80C3935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="158">
   <si>
     <t>Name</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Faustus' Spare Room Key</t>
   </si>
   <si>
-    <t>Journal "tlvoea_Errant_Wife", 20; Goodbye</t>
-  </si>
-  <si>
     <t>Thank you for safely escorting me back home %PCName! I'm sure Urtiso will have something for you as thanks.</t>
   </si>
   <si>
@@ -406,9 +403,6 @@
     <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are could you please let my foolish wife know that her she has a worried wife to come home to.</t>
   </si>
   <si>
-    <t>tlvoea_Errant_Wife.Journal &lt; 20, tlvoea_isAelianaHome == 1</t>
-  </si>
-  <si>
     <t>Aeliana? Oh Urtiso's wife. I last saw her somewhere around Haliwaran. Just head a little east down this ridge and it will be in front of you.</t>
   </si>
   <si>
@@ -451,9 +445,6 @@
     <t>I hope you're better with finding your way round than I am.</t>
   </si>
   <si>
-    <t>tlvoea_Errant_Wife.Journal &lt; 20, tlvoea_isAelianaHome == 0</t>
-  </si>
-  <si>
     <t>spare room</t>
   </si>
   <si>
@@ -490,9 +481,6 @@
     <t>tlvoea_Spare_Room.Journal &gt;= 10; Random100 &lt; 55</t>
   </si>
   <si>
-    <t>tlvoea_Errant_Wife.Journal &gt; 11, tlvoea_Errant_Wife.Journal &lt; 20, Random100 &lt; 45</t>
-  </si>
-  <si>
     <t>I hope she's alright.</t>
   </si>
   <si>
@@ -515,6 +503,24 @@
   </si>
   <si>
     <t>MessageBox "You owe %G gold.", tlvoea_Glob_Rent_Counter</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &gt;= 11, tlvoea_Errant_Wife.Journal &lt; 20, Random100 &lt; 45</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &gt;= 11, tlvoea_Errant_Wife.Journal &lt; 20</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &lt;= 11, tlvoea_isAelianaFollowing == 0, tlvoea_isAelianaHome == 0</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &lt; 20, , tlvoea_isAelianaFollowing == 1, tlvoea_isAelianaHome == 0</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &lt; 20, tlvoea_isAelianaFollowing == 1, tlvoea_isAelianaHome == 1</t>
+  </si>
+  <si>
+    <t>AiWander 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0; SetSpeed 54; set tlvoea_isAelianaFollowing to 0; Journal "tlvoea_Errant_Wife", 20; Goodbye</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1499,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1678,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
@@ -1687,7 +1693,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1695,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1704,7 +1710,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1712,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1726,13 +1732,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1740,13 +1746,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2018,15 +2024,15 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2034,10 +2040,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -2045,10 +2051,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -2144,10 +2150,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
         <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2440,7 +2446,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <v>300</v>
@@ -2457,16 +2463,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -2637,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
   <dimension ref="A2:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,10 +2683,10 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2694,7 +2700,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>63</v>
@@ -2711,10 +2717,10 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2728,10 +2734,10 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2745,13 +2751,13 @@
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2768,10 +2774,10 @@
         <v>78</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>1</v>
       </c>
@@ -2782,13 +2788,13 @@
         <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
         <v>1</v>
       </c>
@@ -2799,13 +2805,13 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2819,13 +2825,13 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2839,10 +2845,10 @@
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2856,10 +2862,10 @@
         <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2873,10 +2879,10 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2890,7 +2896,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2901,13 +2907,13 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3066,16 +3072,16 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
         <v>67</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3083,16 +3089,16 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
         <v>67</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3103,13 +3109,13 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>61</v>
@@ -3123,10 +3129,10 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>62</v>
@@ -3140,16 +3146,16 @@
         <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3160,13 +3166,13 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3177,13 +3183,13 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3194,13 +3200,13 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3211,13 +3217,13 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3228,13 +3234,13 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -4124,7 +4130,7 @@
         <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
         <v>82</v>
@@ -4138,7 +4144,7 @@
         <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
         <v>82</v>
@@ -4336,10 +4342,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
         <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4533,10 +4539,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add: move Aeliana post quest
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88A815D-097F-4A17-BB5C-6363DA18FDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B7A1B5-021D-4F60-B01A-AB510A0383FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="2" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -1720,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
   <dimension ref="A2:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>91</v>
@@ -2379,7 +2379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2709,7 +2709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
   <dimension ref="A2:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add: initial lines for fail routes
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B7A1B5-021D-4F60-B01A-AB510A0383FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405FE1FB-217A-4A3F-A65A-EA720728F119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="188">
   <si>
     <t>Name</t>
   </si>
@@ -226,9 +226,6 @@
     <t>Journal "tlvoea_Errant_Wife", 11</t>
   </si>
   <si>
-    <t>Choice "I'll keep an eye out for her.", 1, "Sorry, I won't be going in that direction.", 2</t>
-  </si>
-  <si>
     <t>Choice = 1</t>
   </si>
   <si>
@@ -379,24 +376,12 @@
     <t>[She sniffs your hand.]</t>
   </si>
   <si>
-    <t>Random100 &lt; 75</t>
-  </si>
-  <si>
-    <t>Random100 &lt; 10</t>
-  </si>
-  <si>
     <t>Random100 &lt; 15</t>
   </si>
   <si>
     <t>Talked to PC == 0, tlvoea_Errant_Wife.Journal &lt; 10</t>
   </si>
   <si>
-    <t>My wife is still out, and so the shop remains closed.</t>
-  </si>
-  <si>
-    <t>Have you found Aeliana?</t>
-  </si>
-  <si>
     <t>AddTopic "spare room"; Journal "tlvoea_Errant_Wife", 100</t>
   </si>
   <si>
@@ -436,9 +421,6 @@
     <t>tlvoea_Spare_Room.Journal &gt;= 10; Random100 &lt; 55</t>
   </si>
   <si>
-    <t>I hope she's alright.</t>
-  </si>
-  <si>
     <t>tlvoea_Glob_Rent_Period</t>
   </si>
   <si>
@@ -469,15 +451,6 @@
     <t>AiWander 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0; SetSpeed 54; set tlvoea_isAelianaFollowing to 0; Journal "tlvoea_Errant_Wife", 20; Goodbye</t>
   </si>
   <si>
-    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are could you please let my foolish wife know that she has a worried wife to come home to.</t>
-  </si>
-  <si>
-    <t>My sweetheart is back! %PCName, thank you for returning her to me. As thanks, if you want it, you can have our spare room. We were originally asking for 100 upfront plus the rent, but I'll waive the upfront just for you.</t>
-  </si>
-  <si>
-    <t>I hope you're better with finding your way around than I am.</t>
-  </si>
-  <si>
     <t>You will? I thank you. What's your name? %PCName? Well, I'll think of some suitable reward for you. Just tell her that she has a worried wife to come home to and she'll get the hint. She could have wandered anywhere so ask any hunters in the area, I think Nedalor Ilves is camped just to the south on the ridge.</t>
   </si>
   <si>
@@ -544,9 +517,6 @@
     <t>Hello %PCName.</t>
   </si>
   <si>
-    <t>Oh hello there! I was just resting after gathering some plant samples for my research. Now that I'm thinking about it, I don't know which way is home. I was rather distracted by a this cute velk and then I stumbled across all these charming guar. I don't suppose you could escort me back to my house near Old Ebonheart? I really hope I don't have a worried wife on my return.</t>
-  </si>
-  <si>
     <t>Talked to PC == 0; tlvoea_Errant_Wife.Journal &lt;= 11, tlvoea_isAelianaFollowing == 0, tlvoea_isAelianaHome == 0</t>
   </si>
   <si>
@@ -587,6 +557,60 @@
   </si>
   <si>
     <t>I have accepted to rent the Faustus' spare room. They've given me the room key, and I must pay a weekly rate of 105 gold.</t>
+  </si>
+  <si>
+    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are could you please let that fool know that she has a worried wife to come home to.</t>
+  </si>
+  <si>
+    <t>Unfortunately Aeliana is still out, and so the shop remains closed.</t>
+  </si>
+  <si>
+    <t>She had better not have gotten into trouble. I don't want to bail her out again.</t>
+  </si>
+  <si>
+    <t>%PCName, thank you for returning her to me. As thanks, if you want it, our spare room is available to rent.</t>
+  </si>
+  <si>
+    <t>Oh hello there! I was just resting after gathering some plant samples for my research. Now that I'm thinking about it, I don't know which way is home. I was rather distracted by this cute velk and then I stumbled across all these charming guar. I don't suppose you could escort me back to my house near Old Ebonheart? I really hope I don't have a worried wife on my return.</t>
+  </si>
+  <si>
+    <t>I hope you're better at finding your way around than I am.</t>
+  </si>
+  <si>
+    <t>Random100 &lt; 80</t>
+  </si>
+  <si>
+    <t>Random100 &lt; 55</t>
+  </si>
+  <si>
+    <t>Random100 &lt; 30</t>
+  </si>
+  <si>
+    <t>*Squeek* [She nuzzles your hand.]</t>
+  </si>
+  <si>
+    <t>Choice = 10</t>
+  </si>
+  <si>
+    <t>Choice = 11</t>
+  </si>
+  <si>
+    <t>You bastard! I will ensure you're death is slow and painful!</t>
+  </si>
+  <si>
+    <t>SetDisposition 0; StartCombat; Goodbye</t>
+  </si>
+  <si>
+    <t>IF isAelianaDead: Choice "I killed her.", 10, "I'm sorry, she's dead.", 11, "Sorry, I won't be going in that direction.", 2 ELSE Choice "I'll keep an eye out for her.", 1, "Sorry, I won't be going in that direction.", 2</t>
+  </si>
+  <si>
+    <t>StartScript "tlvoea_errant_glb_script"; Goodbye</t>
+  </si>
+  <si>
+    <t>Thank you %PCName for… for letting me know. Please leave me.</t>
+  </si>
+  <si>
+    <t>%PCClass, any luck with finding Aeliana?</t>
   </si>
 </sst>
 </file>
@@ -1565,7 +1589,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1720,7 +1744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
   <dimension ref="A2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1750,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
@@ -1759,7 +1783,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1767,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1776,7 +1800,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1784,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1798,13 +1822,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1812,13 +1836,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2090,15 +2114,15 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2106,10 +2130,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4">
         <v>105</v>
@@ -2117,10 +2141,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -2216,10 +2240,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
         <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2512,7 +2536,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8">
         <v>300</v>
@@ -2529,16 +2553,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -2707,10 +2731,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F127"/>
+  <dimension ref="A2:F130"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2740,7 +2764,7 @@
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
@@ -2749,15 +2773,15 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -2766,15 +2790,15 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -2783,15 +2807,15 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
@@ -2800,15 +2824,15 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -2817,13 +2841,13 @@
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2837,15 +2861,15 @@
         <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
@@ -2854,10 +2878,10 @@
         <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2871,15 +2895,15 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
@@ -2888,10 +2912,10 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2905,13 +2929,13 @@
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2925,13 +2949,13 @@
         <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2945,10 +2969,10 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2962,10 +2986,10 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2979,10 +3003,10 @@
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2996,10 +3020,10 @@
         <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3013,10 +3037,10 @@
         <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -3030,15 +3054,15 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
@@ -3047,10 +3071,10 @@
         <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3067,7 +3091,7 @@
         <v>108</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3084,7 +3108,7 @@
         <v>107</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3100,45 +3124,42 @@
       <c r="D23" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F23" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="b">
         <v>1</v>
       </c>
@@ -3146,16 +3167,19 @@
         <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="b">
         <v>1</v>
       </c>
@@ -3163,90 +3187,90 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3257,110 +3281,110 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="F34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F33" s="2" t="s">
+    </row>
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="b">
         <v>1</v>
       </c>
@@ -3368,13 +3392,16 @@
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -3382,33 +3409,36 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="F39" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>127</v>
+        <v>168</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3416,53 +3446,50 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>35</v>
       </c>
-      <c r="C41" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>177</v>
+        <v>122</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3470,19 +3497,19 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>176</v>
+        <v>121</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="b">
         <v>1</v>
       </c>
@@ -3490,16 +3517,16 @@
         <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="b">
         <v>1</v>
       </c>
@@ -3507,101 +3534,140 @@
         <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" t="s">
+        <v>127</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="b">
         <v>0</v>
       </c>
@@ -3921,8 +3987,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F127">
+  <conditionalFormatting sqref="B3:F130">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4395,13 +4476,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4409,13 +4490,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -4423,13 +4504,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
         <v>74</v>
       </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -4610,10 +4691,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4807,10 +4888,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add: give food topic
Update: various lines
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405FE1FB-217A-4A3F-A65A-EA720728F119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ADC464-7B12-4C52-8611-73FD6D67A18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="204">
   <si>
     <t>Name</t>
   </si>
@@ -313,9 +313,6 @@
     <t>I've killed Urtiso Faustus.</t>
   </si>
   <si>
-    <t>NoLore, isAelianaDead</t>
-  </si>
-  <si>
     <t>isUrtisoDead</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
     <t>Choice = 11</t>
   </si>
   <si>
-    <t>You bastard! I will ensure you're death is slow and painful!</t>
-  </si>
-  <si>
     <t>SetDisposition 0; StartCombat; Goodbye</t>
   </si>
   <si>
@@ -611,6 +605,60 @@
   </si>
   <si>
     <t>%PCClass, any luck with finding Aeliana?</t>
+  </si>
+  <si>
+    <t>You bastard! I will ensure that your death is slow and painful!</t>
+  </si>
+  <si>
+    <t>give food</t>
+  </si>
+  <si>
+    <t>[She looks at you expectantly.]</t>
+  </si>
+  <si>
+    <t>if PC Large Kwama Egg &gt;= 1: Choice "Large Kwama Egg", 1; if PC Small Egg &gt;= 1: Choice "Small Kwama Egg", 2; if PC ScribJelly &gt;= 1: Choice "Scrib Jelly", 3; if PC Comberry &gt;= 1; Choice "Comberry", 4</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "food_kwama_egg_01", 1</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "food_kwama_egg_02", 1</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "ingred_scrib_jelly_01", 1</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "ingred_comberry_01", 1</t>
+  </si>
+  <si>
+    <t>[She nibbles away at the berries, and then scurries away. Returning with an item in her mouth that she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>[She licks the jelly, and then scurries away. Returning with an item in her mouth that she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>*Squeek* [She quickly tucks into the egg. When finished she scurries away, returning with an item in her mouth that she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>*SQUEEK* [She starts jumping excitedly as you give her the large egg.] *Squeek* *Squeek* [She excitedly cracks open the egg and devours the gooey innards. When she's satisfied that the empty shell is licked clean she rushes into her pile of cushions, returning with an item in her mouth that she carefully places into your hand.]</t>
+  </si>
+  <si>
+    <t>tlvoea_rattus_script</t>
+  </si>
+  <si>
+    <t>isRattusDead, hasRattusBeenFed</t>
+  </si>
+  <si>
+    <t>NoLore, isAelianaDead, hasMentionedRattus</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &gt;= 100; hasMentionedRattus == 0</t>
+  </si>
+  <si>
+    <t>By the way, have you met Rattus? She spends her time downstairs in her little nook. You might like her!</t>
+  </si>
+  <si>
+    <t>AddTopic "give food"; set hasMentionedRattus to 1</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1637,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1742,10 +1790,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:E34"/>
+  <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1783,7 +1831,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1800,7 +1848,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1808,27 +1856,30 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>198</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>91</v>
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1836,21 +1887,27 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
       </c>
       <c r="C8" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2061,8 +2118,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:E34">
+  <conditionalFormatting sqref="B3:E35">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$C3=TRUE</formula>
     </cfRule>
@@ -2074,7 +2139,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B3:B34" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B3:B35" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2084,7 +2149,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C35:C62</xm:sqref>
+          <xm:sqref>C36:C63</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2114,15 +2179,15 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2130,10 +2195,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4">
         <v>105</v>
@@ -2141,10 +2206,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -2556,7 +2621,7 @@
         <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2731,10 +2796,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F130"/>
+  <dimension ref="A2:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2764,7 +2829,7 @@
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
@@ -2773,15 +2838,15 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -2790,7 +2855,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>61</v>
@@ -2798,7 +2863,7 @@
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -2807,15 +2872,15 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
@@ -2824,15 +2889,15 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -2841,10 +2906,10 @@
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>76</v>
@@ -2861,15 +2926,15 @@
         <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
@@ -2878,10 +2943,10 @@
         <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2895,15 +2960,15 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
@@ -2912,10 +2977,10 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2932,10 +2997,10 @@
         <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2969,10 +3034,10 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2986,10 +3051,10 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3003,10 +3068,10 @@
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3020,10 +3085,10 @@
         <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3037,13 +3102,13 @@
         <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="b">
         <v>1</v>
       </c>
@@ -3054,27 +3119,30 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>155</v>
+        <v>202</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3088,10 +3156,10 @@
         <v>57</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3141,45 +3209,42 @@
       <c r="D24" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F24" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
         <v>35</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="b">
         <v>1</v>
       </c>
@@ -3190,15 +3255,18 @@
         <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
         <v>38</v>
@@ -3207,18 +3275,15 @@
         <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>38</v>
@@ -3230,15 +3295,15 @@
         <v>186</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
@@ -3247,16 +3312,16 @@
         <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="b">
         <v>1</v>
       </c>
@@ -3267,33 +3332,33 @@
         <v>64</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>62</v>
+        <v>135</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>139</v>
+        <v>62</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="b">
         <v>1</v>
       </c>
@@ -3304,13 +3369,16 @@
         <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="b">
         <v>1</v>
       </c>
@@ -3321,16 +3389,13 @@
         <v>64</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="b">
         <v>1</v>
       </c>
@@ -3341,30 +3406,33 @@
         <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>143</v>
+        <v>65</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
         <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3378,33 +3446,30 @@
         <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="b">
         <v>1</v>
       </c>
@@ -3412,16 +3477,19 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="b">
         <v>1</v>
       </c>
@@ -3429,19 +3497,16 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="b">
         <v>1</v>
       </c>
@@ -3449,13 +3514,16 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="F41" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,19 +3531,19 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="b">
         <v>1</v>
       </c>
@@ -3483,16 +3551,16 @@
         <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="b">
         <v>1</v>
       </c>
@@ -3500,33 +3568,33 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="b">
         <v>1</v>
       </c>
@@ -3534,19 +3602,16 @@
         <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="b">
         <v>1</v>
       </c>
@@ -3554,13 +3619,16 @@
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>166</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -3571,16 +3639,16 @@
         <v>38</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="b">
         <v>1</v>
       </c>
@@ -3588,86 +3656,170 @@
         <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
+        <v>187</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" t="s">
+        <v>187</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
+        <v>187</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="b">
         <v>0</v>
       </c>
@@ -4002,8 +4154,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F130">
+  <conditionalFormatting sqref="B3:F135">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4236,7 +4413,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4479,7 +4656,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
         <v>72</v>
@@ -4493,7 +4670,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>72</v>
@@ -4691,10 +4868,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
         <v>96</v>
-      </c>
-      <c r="C3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4888,10 +5065,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
         <v>98</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add: scripted limit to Rattus
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ADC464-7B12-4C52-8611-73FD6D67A18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C3F817-617C-4F85-AB98-0275A63BAAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="206">
   <si>
     <t>Name</t>
   </si>
@@ -659,6 +659,12 @@
   </si>
   <si>
     <t>AddTopic "give food"; set hasMentionedRattus to 1</t>
+  </si>
+  <si>
+    <t>tlvoea_isAelianaFollowing == 1, tlvoea_isAelianaHome == 0</t>
+  </si>
+  <si>
+    <t>I was such a fool following that velk!</t>
   </si>
 </sst>
 </file>
@@ -1793,7 +1799,7 @@
   <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1836,7 +1842,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>82</v>
@@ -1853,7 +1859,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>198</v>
@@ -2796,10 +2802,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F135"/>
+  <dimension ref="A2:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3395,9 +3401,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -3406,16 +3412,13 @@
         <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="b">
         <v>1</v>
       </c>
@@ -3426,30 +3429,33 @@
         <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
         <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3463,33 +3469,30 @@
         <v>64</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="b">
         <v>1</v>
       </c>
@@ -3500,13 +3503,16 @@
         <v>111</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="b">
         <v>1</v>
       </c>
@@ -3517,16 +3523,13 @@
         <v>111</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="b">
         <v>1</v>
       </c>
@@ -3537,10 +3540,13 @@
         <v>111</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>117</v>
+        <v>167</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -3548,19 +3554,19 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
         <v>111</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="b">
         <v>1</v>
       </c>
@@ -3571,13 +3577,13 @@
         <v>111</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="b">
         <v>1</v>
       </c>
@@ -3588,30 +3594,30 @@
         <v>111</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" t="s">
-        <v>126</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="b">
         <v>1</v>
       </c>
@@ -3622,16 +3628,13 @@
         <v>126</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="b">
         <v>1</v>
       </c>
@@ -3642,10 +3645,13 @@
         <v>126</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -3659,13 +3665,13 @@
         <v>126</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="b">
         <v>1</v>
       </c>
@@ -3676,33 +3682,30 @@
         <v>126</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" t="s">
-        <v>187</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="b">
         <v>1</v>
       </c>
@@ -3713,13 +3716,13 @@
         <v>187</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3733,13 +3736,13 @@
         <v>187</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3753,16 +3756,16 @@
         <v>187</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="b">
         <v>1</v>
       </c>
@@ -3773,15 +3776,30 @@
         <v>187</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -4179,8 +4197,13 @@
         <v>0</v>
       </c>
     </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F135">
+  <conditionalFormatting sqref="B3:F136">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add: Rattus levelled items
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C3F817-617C-4F85-AB98-0275A63BAAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E3917-F90D-4AB7-B372-891397E08453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="210">
   <si>
     <t>Name</t>
   </si>
@@ -616,9 +616,6 @@
     <t>[She looks at you expectantly.]</t>
   </si>
   <si>
-    <t>if PC Large Kwama Egg &gt;= 1: Choice "Large Kwama Egg", 1; if PC Small Egg &gt;= 1: Choice "Small Kwama Egg", 2; if PC ScribJelly &gt;= 1: Choice "Scrib Jelly", 3; if PC Comberry &gt;= 1; Choice "Comberry", 4</t>
-  </si>
-  <si>
     <t>Player-&gt;RemoveItem "food_kwama_egg_01", 1</t>
   </si>
   <si>
@@ -664,7 +661,22 @@
     <t>tlvoea_isAelianaFollowing == 1, tlvoea_isAelianaHome == 0</t>
   </si>
   <si>
-    <t>I was such a fool following that velk!</t>
+    <t>[She looks rather full.]</t>
+  </si>
+  <si>
+    <t>rattusBeenFedDay &gt; 0</t>
+  </si>
+  <si>
+    <t>Choice = 99</t>
+  </si>
+  <si>
+    <t>if PC Large Kwama Egg &gt;= 1: Choice "Large Kwama Egg", 1; if PC Small Egg &gt;= 1: Choice "Small Kwama Egg", 2; if PC ScribJelly &gt;= 1: Choice "Scrib Jelly", 3; if PC Comberry &gt;= 1; Choice "Comberry", 4; Choice "Don't give her anything.", 99</t>
+  </si>
+  <si>
+    <t>[Rattus snorts.]</t>
+  </si>
+  <si>
+    <t>I was such a fool following that velk.</t>
   </si>
 </sst>
 </file>
@@ -1837,7 +1849,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1862,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1871,7 +1883,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2802,10 +2814,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F136"/>
+  <dimension ref="A2:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3125,13 +3137,13 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -3403,7 +3415,7 @@
     </row>
     <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -3412,10 +3424,10 @@
         <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3716,10 +3728,10 @@
         <v>187</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>59</v>
@@ -3736,10 +3748,10 @@
         <v>187</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>60</v>
@@ -3756,10 +3768,10 @@
         <v>187</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>66</v>
@@ -3776,16 +3788,16 @@
         <v>187</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="b">
         <v>1</v>
       </c>
@@ -3796,20 +3808,44 @@
         <v>187</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>189</v>
+        <v>208</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>187</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" t="s">
+        <v>187</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -4202,8 +4238,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F136">
+  <conditionalFormatting sqref="B3:F138">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update: various lines to read less clunky
* Update: Fixed green tint on some light sources by creating new lights with lower radius
* Update: balanced rattus rewards
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E3917-F90D-4AB7-B372-891397E08453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650D21AD-4BB7-4695-BC9E-04BF824E9D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="214">
   <si>
     <t>Name</t>
   </si>
@@ -448,9 +448,6 @@
     <t>AiWander 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0; SetSpeed 54; set tlvoea_isAelianaFollowing to 0; Journal "tlvoea_Errant_Wife", 20; Goodbye</t>
   </si>
   <si>
-    <t>You will? I thank you. What's your name? %PCName? Well, I'll think of some suitable reward for you. Just tell her that she has a worried wife to come home to and she'll get the hint. She could have wandered anywhere so ask any hunters in the area, I think Nedalor Ilves is camped just to the south on the ridge.</t>
-  </si>
-  <si>
     <t>Of course, that's alright. She might yet turn up on her own.</t>
   </si>
   <si>
@@ -466,12 +463,6 @@
     <t>Journal "tlvoea_Errant_Wife", 10; AiFollow Player, 0, 0, 0, 0; SetSpeed 75; set tlvoea_isAelianaFollowing to 1</t>
   </si>
   <si>
-    <t>She normally keeps me company when I head out to gather samples, which we normally turn it into a lovely day out. We bring some food, and sometimes even give Rattus a walk! Oh, I'm rambling, I don't suppose you would be so kind as to escort me home?</t>
-  </si>
-  <si>
-    <t>Oh, oh no. She's going to give me an earful! Please %PCName, could you escort me back home.</t>
-  </si>
-  <si>
     <t>Aeliana? Ah right, Urtiso's wife. I last saw her between Haliwaran and Dondril. To get to Haliwaran just head due east down this ridge and it will be in front of you.</t>
   </si>
   <si>
@@ -517,9 +508,6 @@
     <t>Talked to PC == 0; tlvoea_Errant_Wife.Journal &lt;= 11, tlvoea_isAelianaFollowing == 0, tlvoea_isAelianaHome == 0</t>
   </si>
   <si>
-    <t>It's good to see you too %PCName. As you can see I'm still rather lost.</t>
-  </si>
-  <si>
     <t>tlvoea_Errant_Wife.Journal &gt;= 20</t>
   </si>
   <si>
@@ -550,27 +538,15 @@
     <t>Player-&gt;RemoveItem "Gold_001", tlvoea_Glob_Rent_Counter; set tlvoea_Glob_Rent_Counter to 0</t>
   </si>
   <si>
-    <t>It's not much, but it's yours for 105 gold a week, which is 15 gold a night. A very competitive price, I'm sure you'll agree. It has a bed, side table, chest and candle. The landing is also largely yours to do with as we usually keep to ourselves down here.</t>
-  </si>
-  <si>
     <t>I have accepted to rent the Faustus' spare room. They've given me the room key, and I must pay a weekly rate of 105 gold.</t>
   </si>
   <si>
-    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are could you please let that fool know that she has a worried wife to come home to.</t>
-  </si>
-  <si>
     <t>Unfortunately Aeliana is still out, and so the shop remains closed.</t>
   </si>
   <si>
-    <t>She had better not have gotten into trouble. I don't want to bail her out again.</t>
-  </si>
-  <si>
     <t>%PCName, thank you for returning her to me. As thanks, if you want it, our spare room is available to rent.</t>
   </si>
   <si>
-    <t>Oh hello there! I was just resting after gathering some plant samples for my research. Now that I'm thinking about it, I don't know which way is home. I was rather distracted by this cute velk and then I stumbled across all these charming guar. I don't suppose you could escort me back to my house near Old Ebonheart? I really hope I don't have a worried wife on my return.</t>
-  </si>
-  <si>
     <t>I hope you're better at finding your way around than I am.</t>
   </si>
   <si>
@@ -595,9 +571,6 @@
     <t>SetDisposition 0; StartCombat; Goodbye</t>
   </si>
   <si>
-    <t>IF isAelianaDead: Choice "I killed her.", 10, "I'm sorry, she's dead.", 11, "Sorry, I won't be going in that direction.", 2 ELSE Choice "I'll keep an eye out for her.", 1, "Sorry, I won't be going in that direction.", 2</t>
-  </si>
-  <si>
     <t>StartScript "tlvoea_errant_glb_script"; Goodbye</t>
   </si>
   <si>
@@ -616,30 +589,6 @@
     <t>[She looks at you expectantly.]</t>
   </si>
   <si>
-    <t>Player-&gt;RemoveItem "food_kwama_egg_01", 1</t>
-  </si>
-  <si>
-    <t>Player-&gt;RemoveItem "food_kwama_egg_02", 1</t>
-  </si>
-  <si>
-    <t>Player-&gt;RemoveItem "ingred_scrib_jelly_01", 1</t>
-  </si>
-  <si>
-    <t>Player-&gt;RemoveItem "ingred_comberry_01", 1</t>
-  </si>
-  <si>
-    <t>[She nibbles away at the berries, and then scurries away. Returning with an item in her mouth that she puts into your hand.]</t>
-  </si>
-  <si>
-    <t>[She licks the jelly, and then scurries away. Returning with an item in her mouth that she puts into your hand.]</t>
-  </si>
-  <si>
-    <t>*Squeek* [She quickly tucks into the egg. When finished she scurries away, returning with an item in her mouth that she puts into your hand.]</t>
-  </si>
-  <si>
-    <t>*SQUEEK* [She starts jumping excitedly as you give her the large egg.] *Squeek* *Squeek* [She excitedly cracks open the egg and devours the gooey innards. When she's satisfied that the empty shell is licked clean she rushes into her pile of cushions, returning with an item in her mouth that she carefully places into your hand.]</t>
-  </si>
-  <si>
     <t>tlvoea_rattus_script</t>
   </si>
   <si>
@@ -652,9 +601,6 @@
     <t>tlvoea_Errant_Wife.Journal &gt;= 100; hasMentionedRattus == 0</t>
   </si>
   <si>
-    <t>By the way, have you met Rattus? She spends her time downstairs in her little nook. You might like her!</t>
-  </si>
-  <si>
     <t>AddTopic "give food"; set hasMentionedRattus to 1</t>
   </si>
   <si>
@@ -677,6 +623,76 @@
   </si>
   <si>
     <t>I was such a fool following that velk.</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "food_kwama_egg_02", 1; Player-&gt;AddItem "tlvoea_random_rattus_high", 1
+set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "food_kwama_egg_01", 1; Player-&gt;AddItem "tlvoea_random_rattus_med", 1
+set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "ingred_scrib_jelly_01", 1; Player-&gt;AddItem "tlvoea_random_rattus_low", 1
+set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "ingred_comberry_01", 1; Player-&gt;AddItem "tlvoea_random_rattus_low", 1
+set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
+  </si>
+  <si>
+    <t>*SQUEEK* [She starts jumping excitedly as you give her the large egg.] *Squeek* *Squeek* [She hurridly cracks open the egg and devours the gooey innards. When she's satisfied that the empty shell is licked clean she rushes into her pile of cushions, returning with an item that she carefully places into your hand.]</t>
+  </si>
+  <si>
+    <t>*Squeek* [She quickly tucks into the egg. When finished she scurries away, returning with an item she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>[She licks the jelly, and then scurries away. Returning with an item that she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>[She nibbles away at the berries, and then scurries away. Returning with an item that she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are, could you please let that fool know that she has a worried wife to come home to.</t>
+  </si>
+  <si>
+    <t>She better not have got into any trouble. I don't want to bail her out again.</t>
+  </si>
+  <si>
+    <t>Oh hello there! I was just resting after gathering some plant samples for my research. Well, that's not entirely true. There was this very cute velk creature that I spotted while gathering and I wanted to pet it, but it kept running away from me. Then it got really far away and I lost it. Now I'm really lost and have no idea how to get back to Old Ebonheart. I don't suppose you could escort me back to my house near the city? I would like to get back soon so as to not have a worried wife on my return.</t>
+  </si>
+  <si>
+    <t>It's good to see you too %PCName. As you can see I'm still rather lost. At least these charming guar are here to keep me company.</t>
+  </si>
+  <si>
+    <t>By the way, have you met Rattus? She spends her time downstairs in her little nook. You might like her! Sometimes when you giver her food she'll give you something in return. Though I have no idea where she gets all of those objects as she never goes out.</t>
+  </si>
+  <si>
+    <t>You will? I thank you. What's your name? %PCName? Well, I'll think of some suitable reward for you. Just tell her that she has a worried wife to come home to and she'll get the hint. She could have wandered anywhere so ask any hunters in the area. I think Nedalor Ilves is camped just to the south on the ridge.</t>
+  </si>
+  <si>
+    <t>She normally keeps me company when I head out to gather samples, which we normally turn it into a lovely day out. We bring some food, and sometimes even give Rattus a walk! Oh, I'm sorry I'm rambling. If you help me I'm sure Urtiso will give you something as a reward.</t>
+  </si>
+  <si>
+    <t>Oh, oh no. She's going to give me an earful! Please %PCName, could you escort me back home right away.</t>
+  </si>
+  <si>
+    <t>It's not much, but it's yours for 105 gold a week. That comes to 15 gold a night. A very competitive price, I'm sure you'll agree. It has a bed, side table, chest and candle. The landing is also largely yours to do with as we usually keep to ourselves down here.</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal == 100</t>
+  </si>
+  <si>
+    <t>tlvoea_isAelianaDead == 1</t>
+  </si>
+  <si>
+    <t>You have a strange look on your face. Do you know something?</t>
+  </si>
+  <si>
+    <t>Choice "I killed her.", 10, "I'm sorry, she's dead.", 11, "Sorry, it's nothing.", 2</t>
+  </si>
+  <si>
+    <t>Choice "I'll keep an eye out for her.", 1, "Sorry, I won't be going in that direction.", 2</t>
   </si>
 </sst>
 </file>
@@ -1849,7 +1865,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1874,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1883,7 +1899,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2639,7 +2655,7 @@
         <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2814,10 +2830,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F138"/>
+  <dimension ref="A2:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2856,7 +2872,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>109</v>
@@ -2873,7 +2889,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>61</v>
@@ -2890,7 +2906,7 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>127</v>
@@ -2907,7 +2923,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>128</v>
@@ -2924,7 +2940,7 @@
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>110</v>
@@ -2944,13 +2960,13 @@
         <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>1</v>
       </c>
@@ -2961,10 +2977,10 @@
         <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2978,7 +2994,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>129</v>
@@ -2995,7 +3011,7 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>130</v>
@@ -3052,10 +3068,10 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3069,10 +3085,10 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3086,10 +3102,10 @@
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3103,10 +3119,10 @@
         <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3120,13 +3136,13 @@
         <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="b">
         <v>1</v>
       </c>
@@ -3137,13 +3153,13 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -3157,10 +3173,10 @@
         <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3174,7 +3190,7 @@
         <v>57</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>108</v>
@@ -3194,7 +3210,7 @@
         <v>107</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3211,7 +3227,7 @@
         <v>106</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3228,7 +3244,7 @@
         <v>105</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3273,7 +3289,7 @@
         <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>58</v>
@@ -3293,7 +3309,7 @@
         <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>60</v>
@@ -3310,13 +3326,13 @@
         <v>64</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3330,16 +3346,16 @@
         <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="b">
         <v>1</v>
       </c>
@@ -3350,16 +3366,16 @@
         <v>64</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>135</v>
+        <v>211</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="b">
         <v>1</v>
       </c>
@@ -3370,33 +3386,33 @@
         <v>64</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>62</v>
+        <v>134</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
         <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="b">
         <v>1</v>
       </c>
@@ -3407,13 +3423,16 @@
         <v>64</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="b">
         <v>1</v>
       </c>
@@ -3424,13 +3443,13 @@
         <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>209</v>
+        <v>136</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="b">
         <v>1</v>
       </c>
@@ -3441,16 +3460,13 @@
         <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="b">
         <v>1</v>
       </c>
@@ -3461,30 +3477,33 @@
         <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
         <v>64</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>141</v>
+        <v>207</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3498,33 +3517,30 @@
         <v>64</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F40" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="b">
         <v>1</v>
       </c>
@@ -3535,13 +3551,16 @@
         <v>111</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="b">
         <v>1</v>
       </c>
@@ -3552,16 +3571,13 @@
         <v>111</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="b">
         <v>1</v>
       </c>
@@ -3572,10 +3588,13 @@
         <v>111</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>117</v>
+        <v>208</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3583,19 +3602,19 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C44" t="s">
         <v>111</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="b">
         <v>1</v>
       </c>
@@ -3606,13 +3625,13 @@
         <v>111</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="b">
         <v>1</v>
       </c>
@@ -3623,30 +3642,30 @@
         <v>111</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" t="s">
-        <v>126</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="b">
         <v>1</v>
       </c>
@@ -3657,16 +3676,13 @@
         <v>126</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="b">
         <v>1</v>
       </c>
@@ -3677,10 +3693,13 @@
         <v>126</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -3694,13 +3713,13 @@
         <v>126</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="b">
         <v>1</v>
       </c>
@@ -3711,33 +3730,30 @@
         <v>126</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="b">
         <v>1</v>
       </c>
@@ -3745,19 +3761,19 @@
         <v>41</v>
       </c>
       <c r="C53" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="b">
         <v>1</v>
       </c>
@@ -3765,19 +3781,19 @@
         <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="b">
         <v>1</v>
       </c>
@@ -3785,19 +3801,19 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="b">
         <v>1</v>
       </c>
@@ -3805,13 +3821,16 @@
         <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>206</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -3822,16 +3841,16 @@
         <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="b">
         <v>1</v>
       </c>
@@ -3839,18 +3858,30 @@
         <v>41</v>
       </c>
       <c r="C58" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" t="s">
+        <v>178</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -4248,8 +4279,13 @@
         <v>0</v>
       </c>
     </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F138">
+  <conditionalFormatting sqref="B3:F139">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4258,7 +4294,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D1:D1048576" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D33:D1048576 D1:D32" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
       <formula1>512</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add: simplified failure routes
Add: axe reward
Add: disposition increases
Update: rent counter to long
Update: stopping global rent script
Update: Nedalor will mark Dondril on the map
Update: scrapped levelled rewards as it does not function cleanly in dialogue
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650D21AD-4BB7-4695-BC9E-04BF824E9D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2013DED4-E0C9-43CE-BD5B-45402DC44289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="216">
   <si>
     <t>Name</t>
   </si>
@@ -379,9 +379,6 @@
     <t>Talked to PC == 0, tlvoea_Errant_Wife.Journal &lt; 10</t>
   </si>
   <si>
-    <t>AddTopic "spare room"; Journal "tlvoea_Errant_Wife", 100</t>
-  </si>
-  <si>
     <t>spare room</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>I think having you stay with us would be wonderful!</t>
   </si>
   <si>
-    <t>Good, here's your key. It's upstairs and at the end of the landing. As for your rent please come to me to pay it, but don't worry about needing to do so everyday. I understand that you're a busy %PCClass, so I'll keep track of what you owe between visits.</t>
-  </si>
-  <si>
     <t>Not a problem. If you change your mind do speak to me again.</t>
   </si>
   <si>
@@ -445,27 +439,15 @@
     <t>tlvoea_Errant_Wife.Journal &lt; 20, tlvoea_isAelianaFollowing == 1, tlvoea_isAelianaHome == 1</t>
   </si>
   <si>
-    <t>AiWander 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0; SetSpeed 54; set tlvoea_isAelianaFollowing to 0; Journal "tlvoea_Errant_Wife", 20; Goodbye</t>
-  </si>
-  <si>
     <t>Of course, that's alright. She might yet turn up on her own.</t>
   </si>
   <si>
-    <t>I love her, but she can be so foolish and take far too many risks. I swear I'm going grey early because of her. It's been longer than usual and I'm getting worried. I've already gone out and I can't find her in the usual places so I think she's gone further out, probably gotten lost or distracted by something cute. Would you be able to find her?</t>
-  </si>
-  <si>
-    <t>How wonderful! My house is just outside Old Ebonheart, which you can't miss as it's just a little ways down the road from the gate. Lead the way!</t>
-  </si>
-  <si>
     <t>That's ok. Maybe I'll be able to make my own way back.</t>
   </si>
   <si>
     <t>Journal "tlvoea_Errant_Wife", 10; AiFollow Player, 0, 0, 0, 0; SetSpeed 75; set tlvoea_isAelianaFollowing to 1</t>
   </si>
   <si>
-    <t>Aeliana? Ah right, Urtiso's wife. I last saw her between Haliwaran and Dondril. To get to Haliwaran just head due east down this ridge and it will be in front of you.</t>
-  </si>
-  <si>
     <t>AiFollow Player, 0, 0, 0, 0; SetSpeed 75; set tlvoea_isAelianaFollowing to 1; Goodbye</t>
   </si>
   <si>
@@ -544,9 +526,6 @@
     <t>Unfortunately Aeliana is still out, and so the shop remains closed.</t>
   </si>
   <si>
-    <t>%PCName, thank you for returning her to me. As thanks, if you want it, our spare room is available to rent.</t>
-  </si>
-  <si>
     <t>I hope you're better at finding your way around than I am.</t>
   </si>
   <si>
@@ -562,27 +541,9 @@
     <t>*Squeek* [She nuzzles your hand.]</t>
   </si>
   <si>
-    <t>Choice = 10</t>
-  </si>
-  <si>
-    <t>Choice = 11</t>
-  </si>
-  <si>
-    <t>SetDisposition 0; StartCombat; Goodbye</t>
-  </si>
-  <si>
-    <t>StartScript "tlvoea_errant_glb_script"; Goodbye</t>
-  </si>
-  <si>
-    <t>Thank you %PCName for… for letting me know. Please leave me.</t>
-  </si>
-  <si>
     <t>%PCClass, any luck with finding Aeliana?</t>
   </si>
   <si>
-    <t>You bastard! I will ensure that your death is slow and painful!</t>
-  </si>
-  <si>
     <t>give food</t>
   </si>
   <si>
@@ -625,74 +586,119 @@
     <t>I was such a fool following that velk.</t>
   </si>
   <si>
-    <t>Player-&gt;RemoveItem "food_kwama_egg_02", 1; Player-&gt;AddItem "tlvoea_random_rattus_high", 1
+    <t>*SQUEEK* [She starts jumping excitedly as you give her the large egg.] *Squeek* *Squeek* [She hurridly cracks open the egg and devours the gooey innards. When she's satisfied that the empty shell is licked clean she rushes into her pile of cushions, returning with an item that she carefully places into your hand.]</t>
+  </si>
+  <si>
+    <t>*Squeek* [She quickly tucks into the egg. When finished she scurries away, returning with an item she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>[She licks the jelly, and then scurries away. Returning with an item that she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>[She nibbles away at the berries, and then scurries away. Returning with an item that she puts into your hand.]</t>
+  </si>
+  <si>
+    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are, could you please let that fool know that she has a worried wife to come home to.</t>
+  </si>
+  <si>
+    <t>She better not have got into any trouble. I don't want to bail her out again.</t>
+  </si>
+  <si>
+    <t>It's good to see you too %PCName. As you can see I'm still rather lost. At least these charming guar are here to keep me company.</t>
+  </si>
+  <si>
+    <t>By the way, have you met Rattus? She spends her time downstairs in her little nook. You might like her! Sometimes when you giver her food she'll give you something in return. Though I have no idea where she gets all of those objects as she never goes out.</t>
+  </si>
+  <si>
+    <t>You will? I thank you. What's your name? %PCName? Well, I'll think of some suitable reward for you. Just tell her that she has a worried wife to come home to and she'll get the hint. She could have wandered anywhere so ask any hunters in the area. I think Nedalor Ilves is camped just to the south on the ridge.</t>
+  </si>
+  <si>
+    <t>Oh, oh no. She's going to give me an earful! Please %PCName, could you escort me back home right away.</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal == 100</t>
+  </si>
+  <si>
+    <t>Choice "I'll keep an eye out for her.", 1, "Sorry, I won't be going in that direction.", 2</t>
+  </si>
+  <si>
+    <t>tlvoea_Aeliana Faustus.Dead == 1</t>
+  </si>
+  <si>
+    <t>She is? That's… Thank you %PCName for… for letting me know. Please leave me now. I need to prepare for whatever is next.</t>
+  </si>
+  <si>
+    <t>No. No talking. I want to be left alone.</t>
+  </si>
+  <si>
+    <t>I can't believe she's gone.</t>
+  </si>
+  <si>
+    <t>AiWander 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0; SetSpeed 54; set tlvoea_isAelianaFollowing to 0; ModDisposition 10; Journal "tlvoea_Errant_Wife", 20; Goodbye</t>
+  </si>
+  <si>
+    <t>tlvoea_Urtiso Faustus.Dead == 1</t>
+  </si>
+  <si>
+    <t>What!? How could this be!? I should never ever have wondered so far. She would still… [She's no longer responding to you.]</t>
+  </si>
+  <si>
+    <t>Empty for tracking pre-quest kills</t>
+  </si>
+  <si>
+    <t>Journal tlvoea_Errant_Wife, 400; Goodbye</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal == 400, tlvoea_Aeliana Faustus.Dead == 1</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal == 400; tlvoea_Urtiso Faustus.Dead == 1</t>
+  </si>
+  <si>
+    <t>Aeliana? Ah right, Urtiso's wife. I last saw her between Haliwaran and Dondril. To get to Haliwaran just head due east down this ridge and it will be in front of you. Dondril is just south of there. Here, I'll mark it on your map.</t>
+  </si>
+  <si>
+    <t>ShowMap "Dondril"</t>
+  </si>
+  <si>
+    <t>Player-&gt;RemoveItem "ingred_comberry_01", 1; Player-&gt;AddItem "Gold_001", 1
 set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
   </si>
   <si>
-    <t>Player-&gt;RemoveItem "food_kwama_egg_01", 1; Player-&gt;AddItem "tlvoea_random_rattus_med", 1
+    <t>Player-&gt;RemoveItem "ingred_scrib_jelly_01", 1; Player-&gt;AddItem "Gold_001", 1
 set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
   </si>
   <si>
-    <t>Player-&gt;RemoveItem "ingred_scrib_jelly_01", 1; Player-&gt;AddItem "tlvoea_random_rattus_low", 1
+    <t>Player-&gt;RemoveItem "food_kwama_egg_01", 1; Player-&gt;AddItem "p_dispel_s", 1
 set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
   </si>
   <si>
-    <t>Player-&gt;RemoveItem "ingred_comberry_01", 1; Player-&gt;AddItem "tlvoea_random_rattus_low", 1
+    <t>Player-&gt;RemoveItem "food_kwama_egg_02", 1; Player-&gt;AddItem "p_reflection_s", 1
 set tlvoea_rattusNextFeedDay to ( DaysPassed + 1 )</t>
   </si>
   <si>
-    <t>*SQUEEK* [She starts jumping excitedly as you give her the large egg.] *Squeek* *Squeek* [She hurridly cracks open the egg and devours the gooey innards. When she's satisfied that the empty shell is licked clean she rushes into her pile of cushions, returning with an item that she carefully places into your hand.]</t>
-  </si>
-  <si>
-    <t>*Squeek* [She quickly tucks into the egg. When finished she scurries away, returning with an item she puts into your hand.]</t>
-  </si>
-  <si>
-    <t>[She licks the jelly, and then scurries away. Returning with an item that she puts into your hand.]</t>
-  </si>
-  <si>
-    <t>[She nibbles away at the berries, and then scurries away. Returning with an item that she puts into your hand.]</t>
-  </si>
-  <si>
-    <t>Yes yes, a hello to you too. If you're looking to buy then I'm sorry to say that Aeliana is currently out. Wait, are you heading out into the wilderness? If you are, could you please let that fool know that she has a worried wife to come home to.</t>
-  </si>
-  <si>
-    <t>She better not have got into any trouble. I don't want to bail her out again.</t>
-  </si>
-  <si>
-    <t>Oh hello there! I was just resting after gathering some plant samples for my research. Well, that's not entirely true. There was this very cute velk creature that I spotted while gathering and I wanted to pet it, but it kept running away from me. Then it got really far away and I lost it. Now I'm really lost and have no idea how to get back to Old Ebonheart. I don't suppose you could escort me back to my house near the city? I would like to get back soon so as to not have a worried wife on my return.</t>
-  </si>
-  <si>
-    <t>It's good to see you too %PCName. As you can see I'm still rather lost. At least these charming guar are here to keep me company.</t>
-  </si>
-  <si>
-    <t>By the way, have you met Rattus? She spends her time downstairs in her little nook. You might like her! Sometimes when you giver her food she'll give you something in return. Though I have no idea where she gets all of those objects as she never goes out.</t>
-  </si>
-  <si>
-    <t>You will? I thank you. What's your name? %PCName? Well, I'll think of some suitable reward for you. Just tell her that she has a worried wife to come home to and she'll get the hint. She could have wandered anywhere so ask any hunters in the area. I think Nedalor Ilves is camped just to the south on the ridge.</t>
-  </si>
-  <si>
-    <t>She normally keeps me company when I head out to gather samples, which we normally turn it into a lovely day out. We bring some food, and sometimes even give Rattus a walk! Oh, I'm sorry I'm rambling. If you help me I'm sure Urtiso will give you something as a reward.</t>
-  </si>
-  <si>
-    <t>Oh, oh no. She's going to give me an earful! Please %PCName, could you escort me back home right away.</t>
-  </si>
-  <si>
-    <t>It's not much, but it's yours for 105 gold a week. That comes to 15 gold a night. A very competitive price, I'm sure you'll agree. It has a bed, side table, chest and candle. The landing is also largely yours to do with as we usually keep to ourselves down here.</t>
-  </si>
-  <si>
-    <t>tlvoea_Errant_Wife.Journal == 100</t>
-  </si>
-  <si>
-    <t>tlvoea_isAelianaDead == 1</t>
-  </si>
-  <si>
-    <t>You have a strange look on your face. Do you know something?</t>
-  </si>
-  <si>
-    <t>Choice "I killed her.", 10, "I'm sorry, she's dead.", 11, "Sorry, it's nothing.", 2</t>
-  </si>
-  <si>
-    <t>Choice "I'll keep an eye out for her.", 1, "Sorry, I won't be going in that direction.", 2</t>
+    <t>%PCName, thank you for returning her to me. First of all, I'd like you to have my old axe. I hope it proves as reliable for you as it was for me. Secondly, if you want it, our spare room is available to rent.</t>
+  </si>
+  <si>
+    <t>Player-&gt;AddItem "steel axe", 1; AddTopic "spare room"; ModDisposition 15; Journal "tlvoea_Errant_Wife", 100</t>
+  </si>
+  <si>
+    <t>Oh hello there! I was just resting after gathering some plant samples for my research. Well, that's not entirely true. There was this very cute velk creature that I spotted and I wanted to pet it, but it kept running away from me. Then it got really far away and I lost it. Now I'm really lost and have no idea how to get back to Old Ebonheart. I don't suppose you could escort me back to my house near the city? I would like to get back soon so as to not have a worried wife on my return.</t>
+  </si>
+  <si>
+    <t>I love her, but she can be so foolish and take far too many risks. I swear I'm going grey early because of her! It's been longer than usual and I'm getting worried. I've already checked in the usual places near here so I think she's gone further out, probably gotten lost or distracted by something cute. Would you be able to find her?</t>
+  </si>
+  <si>
+    <t>How wonderful! My house is just outside Old Ebonheart, which you can't miss as it's only a little ways down the road from the gate. Lead the way!</t>
+  </si>
+  <si>
+    <t>She normally keeps me company when I head out to gather samples, which we then turn it into a lovely day out. We bring some food, and sometimes even give Rattus a walk! Oh, I'm sorry I'm rambling. If you help me I'm sure Urtiso will give you something as a reward.</t>
+  </si>
+  <si>
+    <t>It's not much, but it's yours for 105 gold a week. That comes to 15 a night. A very competitive price, I'm sure you'll agree. It has a bed, side table, chest and candle. The landing is also largely yours to do with as we usually keep to ourselves down here.</t>
+  </si>
+  <si>
+    <t>Good, here's your key. It's upstairs and at the end of the landing. As for your rent please come to me to pay it, but don't worry about needing to do so every week. I understand that you're a busy %PCClass, so I'll keep track of what you owe between visits.</t>
   </si>
 </sst>
 </file>
@@ -1827,7 +1833,7 @@
   <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1865,7 +1871,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1890,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1899,7 +1905,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2218,7 +2224,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
         <v>91</v>
@@ -2229,7 +2235,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
         <v>91</v>
@@ -2240,7 +2246,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
@@ -2500,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2647,29 +2653,41 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2784,6 +2802,11 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2796,7 +2819,7 @@
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:F5 B6:F33">
+  <conditionalFormatting sqref="C3:F5 B6:F34">
     <cfRule type="expression" dxfId="17" priority="3">
       <formula>$F3="END"</formula>
     </cfRule>
@@ -2820,7 +2843,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F6 F7:F33</xm:sqref>
+          <xm:sqref>F3:F6 F7:F34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2830,10 +2853,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F139"/>
+  <dimension ref="A2:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2872,7 +2895,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>109</v>
@@ -2889,7 +2912,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>61</v>
@@ -2906,10 +2929,10 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2923,13 +2946,13 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
         <v>1</v>
       </c>
@@ -2940,16 +2963,16 @@
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>110</v>
+        <v>209</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
         <v>1</v>
       </c>
@@ -2960,30 +2983,33 @@
         <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>154</v>
+        <v>193</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>202</v>
+        <v>148</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
         <v>1</v>
       </c>
@@ -2994,10 +3020,10 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3011,13 +3037,13 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
         <v>1</v>
       </c>
@@ -3028,16 +3054,13 @@
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="b">
         <v>1</v>
       </c>
@@ -3048,16 +3071,16 @@
         <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
         <v>1</v>
       </c>
@@ -3068,13 +3091,16 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>142</v>
+        <v>77</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="b">
         <v>1</v>
       </c>
@@ -3085,10 +3111,13 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>141</v>
+        <v>194</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>148</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3102,10 +3131,10 @@
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3119,10 +3148,10 @@
         <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3136,13 +3165,13 @@
         <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="b">
         <v>1</v>
       </c>
@@ -3153,16 +3182,13 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>184</v>
+        <v>137</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="b">
         <v>1</v>
       </c>
@@ -3173,27 +3199,30 @@
         <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3201,16 +3230,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
         <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3224,10 +3253,10 @@
         <v>57</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>106</v>
+        <v>163</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3241,10 +3270,10 @@
         <v>57</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3258,64 +3287,61 @@
         <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="b">
         <v>1</v>
       </c>
@@ -3326,16 +3352,16 @@
         <v>64</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>173</v>
+        <v>58</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="b">
         <v>1</v>
       </c>
@@ -3346,13 +3372,10 @@
         <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3366,13 +3389,13 @@
         <v>64</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3386,10 +3409,10 @@
         <v>64</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>134</v>
+        <v>211</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>61</v>
@@ -3423,10 +3446,10 @@
         <v>64</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>66</v>
@@ -3443,7 +3466,7 @@
         <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>67</v>
@@ -3460,13 +3483,16 @@
         <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>191</v>
+        <v>197</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="b">
         <v>1</v>
       </c>
@@ -3477,16 +3503,13 @@
         <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>65</v>
+        <v>178</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="b">
         <v>1</v>
       </c>
@@ -3497,33 +3520,36 @@
         <v>64</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
         <v>64</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>138</v>
+        <v>188</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="b">
         <v>1</v>
       </c>
@@ -3534,33 +3560,33 @@
         <v>64</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F41" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="b">
         <v>1</v>
       </c>
@@ -3568,16 +3594,19 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>116</v>
+        <v>215</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="b">
         <v>1</v>
       </c>
@@ -3585,19 +3614,16 @@
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="b">
         <v>1</v>
       </c>
@@ -3605,13 +3631,16 @@
         <v>38</v>
       </c>
       <c r="C44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="F44" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3619,19 +3648,19 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="b">
         <v>1</v>
       </c>
@@ -3639,16 +3668,16 @@
         <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="b">
         <v>1</v>
       </c>
@@ -3656,33 +3685,33 @@
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="F48" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="b">
         <v>1</v>
       </c>
@@ -3690,19 +3719,16 @@
         <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="b">
         <v>1</v>
       </c>
@@ -3710,13 +3736,16 @@
         <v>38</v>
       </c>
       <c r="C50" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -3727,16 +3756,16 @@
         <v>38</v>
       </c>
       <c r="C51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="b">
         <v>1</v>
       </c>
@@ -3744,36 +3773,33 @@
         <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>178</v>
+        <v>124</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="b">
         <v>1</v>
       </c>
@@ -3781,16 +3807,16 @@
         <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3801,16 +3827,16 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3821,19 +3847,19 @@
         <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="b">
         <v>1</v>
       </c>
@@ -3841,13 +3867,16 @@
         <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3858,16 +3887,16 @@
         <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="b">
         <v>1</v>
       </c>
@@ -3875,18 +3904,30 @@
         <v>41</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -4284,8 +4325,13 @@
         <v>0</v>
       </c>
     </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F139">
+  <conditionalFormatting sqref="B3:F140">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4294,7 +4340,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D33:D1048576 D1:D32" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D1:D1048576" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
       <formula1>512</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add: homebrew potion planning
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2013DED4-E0C9-43CE-BD5B-45402DC44289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AE5C2-E703-4711-8C2D-3EA5C3C87C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="234">
   <si>
     <t>Name</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>Rat</t>
-  </si>
-  <si>
-    <t>Potion</t>
   </si>
   <si>
     <t>Aeliana's Homebrew</t>
@@ -699,6 +696,63 @@
   </si>
   <si>
     <t>Good, here's your key. It's upstairs and at the end of the landing. As for your rent please come to me to pay it, but don't worry about needing to do so every week. I understand that you're a busy %PCClass, so I'll keep track of what you owe between visits.</t>
+  </si>
+  <si>
+    <t>If OnPCEquip: MsgBox "Sure?"; On Yes PositionCell outside of menu</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>AddTopic "Aeliana's homebrew"; set hasMentionedHomebrew to 1</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &gt;= 100; tlvoea_Spare_Room.Journal &gt;= 10; hasMentionedHomebrew == 0</t>
+  </si>
+  <si>
+    <t>There you are %PCName! I've been thinking about how I could thank you properly for escorting me, and I think I have it! I've been cooking up a special Aeliana's homebrew for you!</t>
+  </si>
+  <si>
+    <t>Aeliana's homebrew</t>
+  </si>
+  <si>
+    <t>hasMentionedHomebrew == 1</t>
+  </si>
+  <si>
+    <t>Oh yes! A quick swig of this and it'll whisk you back here nice and safe! Would you like a bottle?</t>
+  </si>
+  <si>
+    <t>set hasMentionedHomebrew to 2; Choice "Please.", 1, "No thank you.", 2</t>
+  </si>
+  <si>
+    <t>Well, it's here ready for you if you change you mind.</t>
+  </si>
+  <si>
+    <t>Wonderful! Here you go! If you need more just ask. Though I can only make one every couple of days.</t>
+  </si>
+  <si>
+    <t>hasMentionedHomebrew == 2</t>
+  </si>
+  <si>
+    <t>Choice "Please.", 1, "No thank you.", 2</t>
+  </si>
+  <si>
+    <t>Interested? I still have that bottle for you.</t>
+  </si>
+  <si>
+    <t>hasMentionedHomebrew == 3</t>
+  </si>
+  <si>
+    <t>Here's another for you. If you need more please give me a couple of days.</t>
+  </si>
+  <si>
+    <t>set hasMentionedHomebrew to 4; Player-&gt;AddItem "tlvoea_homebrew", 1</t>
+  </si>
+  <si>
+    <t>Please give me a little longer as my homebrew's take some time.</t>
+  </si>
+  <si>
+    <t>hasMentionedHomebrew == 4</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1731,7 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1833,7 +1887,7 @@
   <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1862,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
@@ -1871,7 +1925,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1879,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1888,7 +1942,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1896,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1905,7 +1959,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1913,13 +1967,16 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1927,13 +1984,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1941,13 +1998,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2219,15 +2276,15 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2235,10 +2292,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4">
         <v>105</v>
@@ -2246,10 +2303,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -2345,10 +2402,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
         <v>78</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2544,13 +2601,13 @@
         <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -2564,13 +2621,13 @@
         <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4">
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -2584,13 +2641,13 @@
         <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2601,13 +2658,13 @@
         <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -2621,13 +2678,13 @@
         <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>200</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -2641,13 +2698,13 @@
         <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8">
         <v>300</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
@@ -2664,7 +2721,7 @@
         <v>400</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -2675,16 +2732,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
         <v>26</v>
@@ -2853,10 +2910,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F140"/>
+  <dimension ref="A2:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2892,13 +2949,13 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2909,13 +2966,13 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2926,13 +2983,13 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2943,13 +3000,13 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2960,16 +3017,16 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2980,16 +3037,16 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3000,13 +3057,13 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3017,13 +3074,13 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3034,13 +3091,13 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3051,13 +3108,13 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3068,16 +3125,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3088,16 +3145,16 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3108,50 +3165,56 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>136</v>
+        <v>219</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>185</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3162,13 +3225,13 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3179,13 +3242,13 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3196,16 +3259,16 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="b">
         <v>1</v>
       </c>
@@ -3213,19 +3276,16 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="b">
         <v>1</v>
       </c>
@@ -3233,13 +3293,13 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3247,16 +3307,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3267,13 +3327,13 @@
         <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3284,7 +3344,7 @@
         <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>106</v>
@@ -3301,7 +3361,7 @@
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>105</v>
@@ -3318,50 +3378,47 @@
         <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F27" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="b">
         <v>1</v>
       </c>
@@ -3369,16 +3426,19 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>130</v>
+        <v>186</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="b">
         <v>1</v>
       </c>
@@ -3386,19 +3446,16 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>199</v>
+        <v>129</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="b">
         <v>1</v>
       </c>
@@ -3406,19 +3463,19 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="b">
         <v>1</v>
       </c>
@@ -3426,36 +3483,36 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="b">
         <v>1</v>
       </c>
@@ -3463,16 +3520,19 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="b">
         <v>1</v>
       </c>
@@ -3480,16 +3540,13 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>199</v>
+        <v>130</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>196</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3500,16 +3557,19 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>178</v>
+        <v>196</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="b">
         <v>1</v>
       </c>
@@ -3517,19 +3577,16 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>65</v>
+        <v>177</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="b">
         <v>1</v>
       </c>
@@ -3537,16 +3594,16 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="F39" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3554,59 +3611,59 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F40" s="2" t="s">
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="b">
         <v>1</v>
       </c>
@@ -3614,16 +3671,19 @@
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>114</v>
+        <v>214</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="b">
         <v>1</v>
       </c>
@@ -3631,19 +3691,16 @@
         <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="b">
         <v>1</v>
       </c>
@@ -3651,13 +3708,16 @@
         <v>38</v>
       </c>
       <c r="C45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="F45" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -3665,19 +3725,19 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="b">
         <v>1</v>
       </c>
@@ -3685,16 +3745,16 @@
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="b">
         <v>1</v>
       </c>
@@ -3702,33 +3762,33 @@
         <v>35</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="b">
         <v>1</v>
       </c>
@@ -3736,19 +3796,16 @@
         <v>38</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="b">
         <v>1</v>
       </c>
@@ -3756,13 +3813,16 @@
         <v>38</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>155</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -3773,16 +3833,16 @@
         <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="b">
         <v>1</v>
       </c>
@@ -3790,242 +3850,338 @@
         <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" t="s">
-        <v>165</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" t="s">
+        <v>220</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" t="s">
+        <v>220</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B55" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" t="s">
-        <v>165</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B56" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" t="s">
-        <v>165</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>67</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" t="s">
+        <v>220</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
         <v>41</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F58" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" t="s">
-        <v>165</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C60" t="s">
-        <v>165</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="b">
         <v>0</v>
       </c>
@@ -4330,8 +4486,43 @@
         <v>0</v>
       </c>
     </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F140">
+  <conditionalFormatting sqref="B3:F147">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4765,7 +4956,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4790,13 +4981,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4804,13 +4995,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4818,13 +5009,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -4832,13 +5023,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
-        <v>74</v>
-      </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -5019,10 +5210,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
         <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5216,10 +5407,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add: homebrew potion and dialogue
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AE5C2-E703-4711-8C2D-3EA5C3C87C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B6B383-19C7-4F7D-BC45-E9BFDF18824C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="236">
   <si>
     <t>Name</t>
   </si>
@@ -554,9 +554,6 @@
   </si>
   <si>
     <t>NoLore, isAelianaDead, hasMentionedRattus</t>
-  </si>
-  <si>
-    <t>tlvoea_Errant_Wife.Journal &gt;= 100; hasMentionedRattus == 0</t>
   </si>
   <si>
     <t>AddTopic "give food"; set hasMentionedRattus to 1</t>
@@ -753,6 +750,15 @@
   </si>
   <si>
     <t>hasMentionedHomebrew == 4</t>
+  </si>
+  <si>
+    <t>tlvoea_Errant_Wife.Journal &gt;= 100; tlvoea_Spare_Room.Journal &gt;= 10; hasMentionedRattus == 0</t>
+  </si>
+  <si>
+    <t>hasMentionedHomebrew == 3; PC has homebrew &gt;= 1</t>
+  </si>
+  <si>
+    <t>Oh! I can see that you already have a bottle of my homebrew. In which case, I'd rather not give you another until you've used that one. In my experiments I had some rather… strange behaviour when there were more than one bottle.</t>
   </si>
 </sst>
 </file>
@@ -1887,7 +1893,7 @@
   <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +1970,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>93</v>
@@ -1976,7 +1982,7 @@
         <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2721,7 +2727,7 @@
         <v>400</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -2910,10 +2916,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F147"/>
+  <dimension ref="A2:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2952,7 +2958,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>108</v>
@@ -2986,7 +2992,7 @@
         <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>124</v>
@@ -3020,10 +3026,10 @@
         <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>75</v>
@@ -3040,13 +3046,13 @@
         <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3063,7 +3069,7 @@
         <v>147</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3077,7 +3083,7 @@
         <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>145</v>
@@ -3094,7 +3100,7 @@
         <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>126</v>
@@ -3131,7 +3137,7 @@
         <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>128</v>
@@ -3168,18 +3174,18 @@
         <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
@@ -3188,18 +3194,18 @@
         <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
@@ -3208,13 +3214,13 @@
         <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3429,7 +3435,7 @@
         <v>63</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>57</v>
@@ -3466,13 +3472,13 @@
         <v>63</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3486,10 +3492,10 @@
         <v>63</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>60</v>
@@ -3523,7 +3529,7 @@
         <v>63</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>131</v>
@@ -3560,13 +3566,13 @@
         <v>63</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3580,10 +3586,10 @@
         <v>63</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3597,7 +3603,7 @@
         <v>63</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>64</v>
@@ -3617,7 +3623,7 @@
         <v>63</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>132</v>
@@ -3637,10 +3643,10 @@
         <v>63</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>84</v>
@@ -3674,7 +3680,7 @@
         <v>109</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>116</v>
@@ -3711,7 +3717,7 @@
         <v>109</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>110</v>
@@ -3878,19 +3884,19 @@
     </row>
     <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B55" t="s">
         <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>58</v>
@@ -3898,16 +3904,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
         <v>35</v>
       </c>
       <c r="C56" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>59</v>
@@ -3915,99 +3921,96 @@
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B57" t="s">
         <v>35</v>
       </c>
       <c r="C57" t="s">
+        <v>219</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
         <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B60" t="s">
         <v>35</v>
       </c>
       <c r="C60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B61" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" t="s">
-        <v>164</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4021,13 +4024,13 @@
         <v>164</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>205</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4041,13 +4044,13 @@
         <v>164</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>204</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4061,16 +4064,16 @@
         <v>164</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="b">
         <v>1</v>
       </c>
@@ -4081,10 +4084,13 @@
         <v>164</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>174</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -4098,13 +4104,13 @@
         <v>164</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="b">
         <v>1</v>
       </c>
@@ -4115,15 +4121,27 @@
         <v>164</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="b">
-        <v>0</v>
+      <c r="E68" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -4521,8 +4539,13 @@
         <v>0</v>
       </c>
     </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F147">
+  <conditionalFormatting sqref="B3:F148">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4987,7 +5010,7 @@
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix: copy issue with dialogue
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B6B383-19C7-4F7D-BC45-E9BFDF18824C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC1F82-05E7-491D-839F-0A27416E2C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -758,7 +758,7 @@
     <t>hasMentionedHomebrew == 3; PC has homebrew &gt;= 1</t>
   </si>
   <si>
-    <t>Oh! I can see that you already have a bottle of my homebrew. In which case, I'd rather not give you another until you've used that one. In my experiments I had some rather… strange behaviour when there were more than one bottle.</t>
+    <t>Oh! I can see that you already have a bottle of my homebrew. In which case, I'd rather not give you another until you've used that one. In my experiments I had some rather… strange behaviour when there were more than one bottle near to each other.</t>
   </si>
 </sst>
 </file>
@@ -2919,7 +2919,7 @@
   <dimension ref="A2:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3959,7 +3959,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add: homebrew timer of 2 days
* Add: rumors to OE & Dondril
* Update: house is illegal to rest
* Update: hitting Rattus starts combat with Urtiso
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\old-ebonheart-apartment\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC1F82-05E7-491D-839F-0A27416E2C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AE32D8-EEB8-43CF-9726-6757E4C765A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="242">
   <si>
     <t>Name</t>
   </si>
@@ -743,9 +743,6 @@
     <t>Here's another for you. If you need more please give me a couple of days.</t>
   </si>
   <si>
-    <t>set hasMentionedHomebrew to 4; Player-&gt;AddItem "tlvoea_homebrew", 1</t>
-  </si>
-  <si>
     <t>Please give me a little longer as my homebrew's take some time.</t>
   </si>
   <si>
@@ -759,6 +756,27 @@
   </si>
   <si>
     <t>Oh! I can see that you already have a bottle of my homebrew. In which case, I'd rather not give you another until you've used that one. In my experiments I had some rather… strange behaviour when there were more than one bottle near to each other.</t>
+  </si>
+  <si>
+    <t>latest rumors</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Disp = 30; Cell == Dondril; tlvoea_Errant_Wife.Journal &lt; 20; (Not Local)T_Local_NoLore == 0; TR_Map == 3; Random100 &lt; 30</t>
+  </si>
+  <si>
+    <t>Disp = 30; Cell == Old Ebonheart; tlvoea_Errant_Wife.Journal &lt; 20; (Not Local)T_Local_NoLore == 0; Random100 &lt; 30; TR_m3_OE_common == 1</t>
+  </si>
+  <si>
+    <t>I heard that Urtiso Fautus has been looking for her wife. Apparently she went missing while out gathering plant samples.</t>
+  </si>
+  <si>
+    <t>A strange Imperial woman has been hanging around the guar along the road to Old Ebonheart. Don't know why she's there, she seems almost lost.</t>
+  </si>
+  <si>
+    <t>set hasMentionedHomebrew to 4; set tlvoea_homebrewReadyDay to ( DaysPassed + 2 ); Player-&gt;AddItem "tlvoea_homebrew", 1</t>
   </si>
 </sst>
 </file>
@@ -2919,7 +2937,7 @@
   <dimension ref="A2:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3220,7 +3238,7 @@
         <v>169</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3882,7 +3900,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="b">
         <v>1</v>
       </c>
@@ -3896,7 +3914,7 @@
         <v>224</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>58</v>
@@ -3970,13 +3988,13 @@
         <v>219</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="b">
         <v>1</v>
       </c>
@@ -3990,7 +4008,7 @@
         <v>229</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>228</v>
@@ -4007,10 +4025,10 @@
         <v>219</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4144,14 +4162,38 @@
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>236</v>
+      </c>
+      <c r="C69" t="s">
+        <v>235</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>236</v>
+      </c>
+      <c r="C70" t="s">
+        <v>235</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>